<commit_message>
SILLi v1.00 Minor Update
Improvements
- Conductivity in the energy equation is the geometric mean of fluid and rock conductivities.
- Result plotting during playback is significantly faster.
- Added an example of an igneous intrusion in a cooled pluton (i.e. no sedimentation or basin evolution involved).

Bug Fixes
- Fixed plotting issue where in some cases whole range of observed data may not be plotted.
- Time step for last point in youngest sedimentary layer corrected.
- Fixed code so that file separators for Mac and Linux systems are recognized and used.
</commit_message>
<xml_diff>
--- a/examples/1d_sill_input_kl178.xlsx
+++ b/examples/1d_sill_input_kl178.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\devel\sill_1d\src\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\GMS\karthik_stuff\SILLi-master\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12105" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Fluid" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>Density (kg/m3)</t>
   </si>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -497,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +516,7 @@
     <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -526,8 +526,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -537,9 +540,12 @@
       <c r="C2">
         <v>3000</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
@@ -553,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -1226,7 +1232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>